<commit_message>
the rest of HUD stuff, added options and dialog modals
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7039706-409A-4F8C-BCC3-9BC850881304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE84A60B-4DBF-485A-A309-FC2464A198B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7455" yWindow="2145" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Key</t>
   </si>
@@ -68,6 +68,48 @@
   </si>
   <si>
     <t>Music from: Kevin Macleod</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
   </si>
 </sst>
 </file>
@@ -403,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,17 +513,73 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
attack bonus distribute mix-up art implemented
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FCE00F-A506-4ABA-8FA4-CC6DE72E529B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EAA5A1-FF4A-43A5-8F64-6CDF3B644625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7455" yWindow="2145" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Key</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>ENTER</t>
+  </si>
+  <si>
+    <t>proceed</t>
+  </si>
+  <si>
+    <t>PROCEED</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +603,14 @@
         <v>31</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
implement victory stuff, added rank icons
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EAA5A1-FF4A-43A5-8F64-6CDF3B644625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BD0111-9EFF-456E-A677-CAA07F9E11EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7455" yWindow="2145" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Key</t>
   </si>
@@ -122,6 +122,30 @@
   </si>
   <si>
     <t>PROCEED</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
+  </si>
+  <si>
+    <t>combo</t>
+  </si>
+  <si>
+    <t>COMBO</t>
+  </si>
+  <si>
+    <t>bonus</t>
+  </si>
+  <si>
+    <t>BONUS</t>
+  </si>
+  <si>
+    <t>perfect</t>
+  </si>
+  <si>
+    <t>PERFECT</t>
   </si>
 </sst>
 </file>
@@ -457,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +635,38 @@
         <v>33</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
lesson background, initial lesson 1 stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BD0111-9EFF-456E-A677-CAA07F9E11EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8D526B-C328-4668-B9C1-36CFC2871BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7455" yWindow="2145" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Key</t>
   </si>
@@ -146,6 +146,24 @@
   </si>
   <si>
     <t>PERFECT</t>
+  </si>
+  <si>
+    <t>Multiply Error:</t>
+  </si>
+  <si>
+    <t>victory_errorMult</t>
+  </si>
+  <si>
+    <t>victory_errorSums</t>
+  </si>
+  <si>
+    <t>Sums Error:</t>
+  </si>
+  <si>
+    <t>victory_score</t>
+  </si>
+  <si>
+    <t>Score:</t>
   </si>
 </sst>
 </file>
@@ -481,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,6 +685,30 @@
         <v>41</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added some illustrations for lesson 1, some changes to lesson 1 flow draft
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8D526B-C328-4668-B9C1-36CFC2871BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF180EE-85E2-4264-A3E3-474FB4B73B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Key</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t>Score:</t>
+  </si>
+  <si>
+    <t>distributiveProperty</t>
+  </si>
+  <si>
+    <t>Distributive Property</t>
+  </si>
+  <si>
+    <t>areaOfRectangle</t>
+  </si>
+  <si>
+    <t>Area of Rectangle</t>
   </si>
 </sst>
 </file>
@@ -499,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,6 +721,22 @@
         <v>47</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
first part of lesson 1 stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF180EE-85E2-4264-A3E3-474FB4B73B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0964B9-B6A6-4B8A-85EE-721CD633BEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Key</t>
   </si>
@@ -176,6 +176,54 @@
   </si>
   <si>
     <t>Area of Rectangle</t>
+  </si>
+  <si>
+    <t>lesson1_distribute_1</t>
+  </si>
+  <si>
+    <t>Multiplying a number of two or more digits can be tricky, but there’s a special trick to make it easier!</t>
+  </si>
+  <si>
+    <t>lesson1_intro_1</t>
+  </si>
+  <si>
+    <t>lesson1_intro_2</t>
+  </si>
+  <si>
+    <t>Let’s take a quick look at a math concept that we will be using for this trick.</t>
+  </si>
+  <si>
+    <t>lesson1_area_1</t>
+  </si>
+  <si>
+    <t>To help visualize this, we will consider these smaller pieces as chunks of a rectangle’s area.</t>
+  </si>
+  <si>
+    <t>lesson1_area_2</t>
+  </si>
+  <si>
+    <t>lesson1_area_3</t>
+  </si>
+  <si>
+    <t>lesson1_area_4</t>
+  </si>
+  <si>
+    <t>As you can see, the rectangle is split into two.</t>
+  </si>
+  <si>
+    <t>Then we compute the area of those two rectangles.</t>
+  </si>
+  <si>
+    <t>And finally, we add these two areas together to get the area of the whole rectangle.</t>
+  </si>
+  <si>
+    <t>Let’s give it a try. Connect these two blobs to initiate the attack!</t>
+  </si>
+  <si>
+    <t>lesson1_connect_1</t>
+  </si>
+  <si>
+    <t>By using the distributive property, we can split up the large number of an equation into smaller pieces.</t>
   </si>
 </sst>
 </file>
@@ -511,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,6 +785,70 @@
         <v>51</v>
       </c>
     </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added warning text for when a mistake happens
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A85BB6-8886-4432-AF56-16A3790F941A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71268D08-540D-42D1-9EB4-D8AA1BF7887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Key</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>Simply click on the boxed number to split it!</t>
+  </si>
+  <si>
+    <t>health_warning</t>
+  </si>
+  <si>
+    <t>Watch out! Once the heart bar is empty, you will have to start over!</t>
   </si>
 </sst>
 </file>
@@ -607,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,145 +825,153 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>78</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added dialogs for bonus stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71268D08-540D-42D1-9EB4-D8AA1BF7887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8E053E-D3F5-4FDD-90CE-026E8EF63684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Key</t>
   </si>
@@ -277,7 +277,91 @@
     <t>health_warning</t>
   </si>
   <si>
-    <t>Watch out! Once the heart bar is empty, you will have to start over!</t>
+    <t>Watch out! Once the health bar is empty, you will have to start over!</t>
+  </si>
+  <si>
+    <t>bonusBlob_1</t>
+  </si>
+  <si>
+    <t>Look, there’s an anomaly blob!</t>
+  </si>
+  <si>
+    <t>bonusBlob_2</t>
+  </si>
+  <si>
+    <t>bonusBlob_3</t>
+  </si>
+  <si>
+    <t>bonusBlob_4</t>
+  </si>
+  <si>
+    <t>Connecting with this blob will allow us to clear out the entire board, and give us a bonus score.</t>
+  </si>
+  <si>
+    <t>Who knows what challenge awaits, so why not give it a try?</t>
+  </si>
+  <si>
+    <t>However, you only have one shot. Do your best!</t>
+  </si>
+  <si>
+    <t>lesson1_attack_distribute_3</t>
+  </si>
+  <si>
+    <t>Since we split the number up in multiples of 10, you are basically multiplying single digit numbers.</t>
+  </si>
+  <si>
+    <t>Just make sure to put the appropriate amount of zeroes at the end!</t>
+  </si>
+  <si>
+    <t>lesson1_attack_eval_3</t>
+  </si>
+  <si>
+    <t>lesson1_attack_eval_4</t>
+  </si>
+  <si>
+    <t>Although we can split the numbers up any ways we want, this is more consistent across most situations.</t>
+  </si>
+  <si>
+    <t>bonus_distribute_mixup_1</t>
+  </si>
+  <si>
+    <t>Looks like the numbers of each area are all mixed up!</t>
+  </si>
+  <si>
+    <t>bonus_distribute_mixup_2</t>
+  </si>
+  <si>
+    <t>bonus_distribute_mixup_3</t>
+  </si>
+  <si>
+    <t>Simply drag the numbers to their appropriate place, and once you are satisfied, press the PROCEED button.</t>
+  </si>
+  <si>
+    <t>Hint: If you look closely at the size of each rectangle, and its associated width, you will know where to put the numbers.</t>
+  </si>
+  <si>
+    <t>bonus_partial_products_1</t>
+  </si>
+  <si>
+    <t>Uh oh, some of the partial products are missing!</t>
+  </si>
+  <si>
+    <t>bonus_partial_products_2</t>
+  </si>
+  <si>
+    <t>bonus_partial_products_3</t>
+  </si>
+  <si>
+    <t>bonus_partial_products_4</t>
+  </si>
+  <si>
+    <t>Use the numpad to fill in the missing numbers, then press the left or right arrows to move to the next one.</t>
+  </si>
+  <si>
+    <t>Once all the missing numbers are filled, press the ENTER button to proceed.</t>
+  </si>
+  <si>
+    <t>Just remember how you split the numbers up into multiples of 10’s like before, and you should have no problem!</t>
   </si>
 </sst>
 </file>
@@ -327,11 +411,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,55 +1011,167 @@
         <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>78</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
double digits lesson implemented
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8E053E-D3F5-4FDD-90CE-026E8EF63684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAE4E32-7052-4839-8FEC-2C3B361C8D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>Key</t>
   </si>
@@ -244,12 +244,6 @@
     <t>lesson1_attack_sums_2</t>
   </si>
   <si>
-    <t>Now we will compute the product of each sub areas by using the numpad to type in the digits.</t>
-  </si>
-  <si>
-    <t>Finally, we add the products together to form the final product!</t>
-  </si>
-  <si>
     <t>Once again, use the numpad to compute each digit of the number.</t>
   </si>
   <si>
@@ -268,12 +262,6 @@
     <t>lesson1_attack_distribute_2</t>
   </si>
   <si>
-    <t>Here we will be splitting the numbers up by multiples of 10.</t>
-  </si>
-  <si>
-    <t>Simply click on the boxed number to split it!</t>
-  </si>
-  <si>
     <t>health_warning</t>
   </si>
   <si>
@@ -307,21 +295,12 @@
     <t>lesson1_attack_distribute_3</t>
   </si>
   <si>
-    <t>Since we split the number up in multiples of 10, you are basically multiplying single digit numbers.</t>
-  </si>
-  <si>
-    <t>Just make sure to put the appropriate amount of zeroes at the end!</t>
-  </si>
-  <si>
     <t>lesson1_attack_eval_3</t>
   </si>
   <si>
     <t>lesson1_attack_eval_4</t>
   </si>
   <si>
-    <t>Although we can split the numbers up any ways we want, this is more consistent across most situations.</t>
-  </si>
-  <si>
     <t>bonus_distribute_mixup_1</t>
   </si>
   <si>
@@ -362,6 +341,87 @@
   </si>
   <si>
     <t>Just remember how you split the numbers up into multiples of 10’s like before, and you should have no problem!</t>
+  </si>
+  <si>
+    <t>Splitting up the numbers this way allows us to simply multiply single digit numbers, and just add the zeroes in the end.</t>
+  </si>
+  <si>
+    <t>Now click on the boxed number to split it!</t>
+  </si>
+  <si>
+    <t>Here we will compute the product of each sub areas by using the numpad to type in the digits.</t>
+  </si>
+  <si>
+    <t>Since we split them up nicely, we only ever have to worry about multiplying single digit numbers.</t>
+  </si>
+  <si>
+    <t>Just remember to add the zero at the end for the number with the denomination of 10!</t>
+  </si>
+  <si>
+    <t>Finally, we add the numbers together to form the final product!</t>
+  </si>
+  <si>
+    <t>Here we will be splitting the numbers up by multiples of 10’s.</t>
+  </si>
+  <si>
+    <t>lesson4_intro_1</t>
+  </si>
+  <si>
+    <t>Here we are at the final stage, with only a handful of blobs left to banish!</t>
+  </si>
+  <si>
+    <t>lesson4_intro_2</t>
+  </si>
+  <si>
+    <t>This time around, we will be multiplying double digit numbers.</t>
+  </si>
+  <si>
+    <t>lesson4_area_1</t>
+  </si>
+  <si>
+    <t>Just as we split the area up horizontally, we can also split it vertically.</t>
+  </si>
+  <si>
+    <t>lesson4_connect_1</t>
+  </si>
+  <si>
+    <t>Now why don’t you give it a try?</t>
+  </si>
+  <si>
+    <t>lesson4_attack_distribute_1</t>
+  </si>
+  <si>
+    <t>Just as you have done up to this point, simply click on the boxed numbers to split them.</t>
+  </si>
+  <si>
+    <t>lesson4_attack_eval_dd_1</t>
+  </si>
+  <si>
+    <t>This time around, you will be multiplying two double digit numbers.</t>
+  </si>
+  <si>
+    <t>lesson4_attack_eval_dd_2</t>
+  </si>
+  <si>
+    <t>lesson4_attack_eval_dd_3</t>
+  </si>
+  <si>
+    <t>Fortunately, they are both multiples of 10.</t>
+  </si>
+  <si>
+    <t>All you need to do is multiply the two non-zero digits, and put two zeroes at the end.</t>
+  </si>
+  <si>
+    <t>lesson4_end_1</t>
+  </si>
+  <si>
+    <t>lesson4_end_2</t>
+  </si>
+  <si>
+    <t>Nice! Even with multiplying double digits, splitting them up allows you to solve them with ease!</t>
+  </si>
+  <si>
+    <t>You will certainly have no problem dealing with the remaining blobs!</t>
   </si>
 </sst>
 </file>
@@ -700,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,10 +972,10 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1003,23 +1063,23 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" t="s">
-        <v>99</v>
+        <v>79</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1027,7 +1087,7 @@
         <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1035,20 +1095,20 @@
         <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
         <v>71</v>
@@ -1059,7 +1119,7 @@
         <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1067,111 +1127,191 @@
         <v>73</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" t="s">
         <v>77</v>
-      </c>
-      <c r="B44" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
         <v>78</v>
-      </c>
-      <c r="B45" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>103</v>
-      </c>
-      <c r="B52" t="s">
-        <v>105</v>
+        <v>126</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>106</v>
-      </c>
-      <c r="B53" t="s">
-        <v>107</v>
+        <v>127</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>108</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>111</v>
+        <v>130</v>
+      </c>
+      <c r="B54" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>109</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
+      </c>
+      <c r="B55" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>110</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>113</v>
+        <v>82</v>
+      </c>
+      <c r="B56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added summary scene, updated rank image for S and SS
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAE4E32-7052-4839-8FEC-2C3B361C8D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3947FE-27A6-4F1D-81B9-799046C3C0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>Key</t>
   </si>
@@ -422,6 +422,42 @@
   </si>
   <si>
     <t>You will certainly have no problem dealing with the remaining blobs!</t>
+  </si>
+  <si>
+    <t>summary_total_score</t>
+  </si>
+  <si>
+    <t>Total Score:</t>
+  </si>
+  <si>
+    <t>level_title_1</t>
+  </si>
+  <si>
+    <t>level_title_2</t>
+  </si>
+  <si>
+    <t>level_title_3</t>
+  </si>
+  <si>
+    <t>level_title_4</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
   </si>
 </sst>
 </file>
@@ -760,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,369 +984,417 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" t="s">
-        <v>81</v>
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
+        <v>134</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
+        <v>137</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
+        <v>138</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
+        <v>139</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>107</v>
+        <v>57</v>
+      </c>
+      <c r="B36" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" t="s">
-        <v>112</v>
+        <v>79</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>119</v>
+        <v>72</v>
+      </c>
+      <c r="B48" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>120</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>121</v>
+        <v>73</v>
+      </c>
+      <c r="B49" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>124</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>125</v>
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>126</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
+      </c>
+      <c r="B52" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>130</v>
-      </c>
-      <c r="B54" t="s">
-        <v>132</v>
+        <v>118</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>131</v>
-      </c>
-      <c r="B55" t="s">
-        <v>133</v>
+        <v>120</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>95</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>97</v>
+        <v>131</v>
+      </c>
+      <c r="B61" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>99</v>
-      </c>
-      <c r="B63" t="s">
-        <v>100</v>
+        <v>84</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>95</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>103</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start background and ui art, removed textmesh pro crap to reduce filesize
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3947FE-27A6-4F1D-81B9-799046C3C0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DEEEC1-30A0-4D97-8111-965030CA8322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>Key</t>
   </si>
@@ -61,15 +61,6 @@
     <t>GO</t>
   </si>
   <si>
-    <t>company</t>
-  </si>
-  <si>
-    <t>RENEGADEWARE</t>
-  </si>
-  <si>
-    <t>Music from: Kevin Macleod</t>
-  </si>
-  <si>
     <t>options</t>
   </si>
   <si>
@@ -458,6 +449,21 @@
   </si>
   <si>
     <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>Made by: RENEGADEWARE, Music from: Kevin MacLeod</t>
   </si>
 </sst>
 </file>
@@ -796,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,250 +854,250 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>135</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" t="s">
-        <v>81</v>
+        <v>131</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>140</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" t="s">
-        <v>53</v>
+        <v>136</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1099,303 +1105,311 @@
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>107</v>
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" t="s">
-        <v>108</v>
+        <v>76</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>116</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
+      </c>
+      <c r="B53" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>122</v>
-      </c>
-      <c r="B56" t="s">
-        <v>123</v>
+        <v>117</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>124</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="B57" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>130</v>
-      </c>
-      <c r="B60" t="s">
-        <v>132</v>
+        <v>124</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B61" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>84</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="B63" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>93</v>
-      </c>
-      <c r="B66" t="s">
-        <v>94</v>
+        <v>83</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>95</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
+      </c>
+      <c r="B67" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>96</v>
-      </c>
-      <c r="B68" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B69" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>101</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="B70" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plan intro and end, some intro stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DEEEC1-30A0-4D97-8111-965030CA8322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164DBD7D-9D93-4B80-99EA-A68FB4FD67A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>Key</t>
   </si>
@@ -34,21 +34,12 @@
     <t>MaxChars</t>
   </si>
   <si>
-    <t>welcome</t>
-  </si>
-  <si>
-    <t>Welcome!</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
     <t>credits_desc</t>
   </si>
   <si>
-    <t>Attack on Blob: Mega Multiply</t>
-  </si>
-  <si>
     <t>ready</t>
   </si>
   <si>
@@ -464,6 +455,21 @@
   </si>
   <si>
     <t>Made by: RENEGADEWARE, Music from: Kevin MacLeod</t>
+  </si>
+  <si>
+    <t>&lt;size=50&gt;Attack on Blob&lt;/size&gt;\nMega Multiply</t>
+  </si>
+  <si>
+    <t>intro_scan_idle</t>
+  </si>
+  <si>
+    <t>Idle</t>
+  </si>
+  <si>
+    <t>intro_scan_danger</t>
+  </si>
+  <si>
+    <t>DANGER!!!</t>
   </si>
 </sst>
 </file>
@@ -802,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,179 +840,173 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>1.5</v>
-      </c>
-      <c r="D2">
-        <v>50</v>
+      <c r="B2" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>39</v>
@@ -1014,98 +1014,98 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>131</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>132</v>
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" t="s">
-        <v>50</v>
+        <v>148</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1113,303 +1113,311 @@
         <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>104</v>
+        <v>62</v>
+      </c>
+      <c r="B43" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" t="s">
-        <v>105</v>
+        <v>73</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>119</v>
-      </c>
-      <c r="B57" t="s">
-        <v>120</v>
+        <v>114</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>121</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>127</v>
-      </c>
-      <c r="B61" t="s">
-        <v>129</v>
+        <v>121</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>81</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="B64" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>90</v>
-      </c>
-      <c r="B67" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>92</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="B68" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>93</v>
-      </c>
-      <c r="B69" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B70" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>98</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+      <c r="B71" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more intro stuff, implement intro
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164DBD7D-9D93-4B80-99EA-A68FB4FD67A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77989E88-C278-42C9-BF6A-64E63C0DF985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2190" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>Key</t>
   </si>
@@ -470,6 +470,48 @@
   </si>
   <si>
     <t>DANGER!!!</t>
+  </si>
+  <si>
+    <t>intro_attack_blob</t>
+  </si>
+  <si>
+    <t>Attack Blob</t>
+  </si>
+  <si>
+    <t>intro_dialog_1</t>
+  </si>
+  <si>
+    <t>intro_dialog_2</t>
+  </si>
+  <si>
+    <t>intro_dialog_3</t>
+  </si>
+  <si>
+    <t>Multiple space blobs have pierced through our dimension!</t>
+  </si>
+  <si>
+    <t>Emergency protocol initiated.</t>
+  </si>
+  <si>
+    <t>We must banish them immediately before they fall down to Earth!</t>
+  </si>
+  <si>
+    <t>intro_attack_1</t>
+  </si>
+  <si>
+    <t>intro_attack_2</t>
+  </si>
+  <si>
+    <t>intro_attack_3</t>
+  </si>
+  <si>
+    <t>With our latest advancements in blobology, we will be deploying Attack Blobs.</t>
+  </si>
+  <si>
+    <t>Our intrepid hero, go forth, and use your mathematical might to banish these invading blobs back to their dimension!</t>
+  </si>
+  <si>
+    <t>These blobs must be made with the power of multiplication, and who better to do it than you!</t>
   </si>
 </sst>
 </file>
@@ -808,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,321 +1144,377 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" t="s">
-        <v>47</v>
+        <v>150</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>153</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>154</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>158</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" t="s">
-        <v>57</v>
+        <v>159</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>73</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>101</v>
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" t="s">
-        <v>68</v>
+        <v>73</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>110</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>111</v>
+        <v>85</v>
+      </c>
+      <c r="B55" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>113</v>
+        <v>86</v>
+      </c>
+      <c r="B56" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>114</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>115</v>
+        <v>66</v>
+      </c>
+      <c r="B57" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>119</v>
+        <v>69</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>122</v>
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>121</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>123</v>
+        <v>108</v>
+      </c>
+      <c r="B61" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>124</v>
-      </c>
-      <c r="B62" t="s">
-        <v>126</v>
+        <v>110</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
-      </c>
-      <c r="B63" t="s">
-        <v>127</v>
+        <v>112</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>76</v>
-      </c>
-      <c r="B64" t="s">
-        <v>77</v>
+        <v>114</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>78</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>81</v>
+        <v>116</v>
+      </c>
+      <c r="B65" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" t="s">
-        <v>88</v>
+        <v>121</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>89</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>91</v>
+        <v>124</v>
+      </c>
+      <c r="B69" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>90</v>
+      </c>
+      <c r="B77" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>93</v>
+      </c>
+      <c r="B78" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>97</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some adjustments to lesson1
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFCB3ED-C399-43F6-85E4-D2D925946455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFE8CAD-D5F0-41C9-B39A-91D6E5A12C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9795" yWindow="2235" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
   <si>
     <t>Key</t>
   </si>
@@ -178,36 +178,18 @@
     <t>lesson1_area_1</t>
   </si>
   <si>
-    <t>To help visualize this, we will consider these smaller pieces as chunks of a rectangle’s area.</t>
-  </si>
-  <si>
     <t>lesson1_area_2</t>
   </si>
   <si>
     <t>lesson1_area_3</t>
   </si>
   <si>
-    <t>lesson1_area_4</t>
-  </si>
-  <si>
-    <t>As you can see, the rectangle is split into two.</t>
-  </si>
-  <si>
-    <t>Then we compute the area of those two rectangles.</t>
-  </si>
-  <si>
-    <t>And finally, we add these two areas together to get the area of the whole rectangle.</t>
-  </si>
-  <si>
     <t>Let’s give it a try. Connect these two blobs to initiate the attack!</t>
   </si>
   <si>
     <t>lesson1_connect_1</t>
   </si>
   <si>
-    <t>By using the distributive property, we can split up the large number of an equation into smaller pieces.</t>
-  </si>
-  <si>
     <t>lesson1_attack_distribute_1</t>
   </si>
   <si>
@@ -530,6 +512,30 @@
   </si>
   <si>
     <t>All the blobs have been banished for good! Earth is safe once more!</t>
+  </si>
+  <si>
+    <t>By using the distributive property, we can split a large number up into smaller pieces.</t>
+  </si>
+  <si>
+    <t>lesson1_distribute_2</t>
+  </si>
+  <si>
+    <t>lesson1_distribute_3</t>
+  </si>
+  <si>
+    <t>In this example, we split up 12 into: 10 and 2. Making it easier to solve the equation.</t>
+  </si>
+  <si>
+    <t>Pay close attention to how the distribution works!</t>
+  </si>
+  <si>
+    <t>To help us visualize this further, consider the product as the area of a rectangle.</t>
+  </si>
+  <si>
+    <t>Splitting the rectangle into two is much similar to how the distributive property works.</t>
+  </si>
+  <si>
+    <t>You compute the area of the two rectangles, and then add them up to get the total area.</t>
   </si>
 </sst>
 </file>
@@ -868,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +907,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -909,7 +915,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,26 +1040,26 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1082,18 +1088,18 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1114,106 +1120,106 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1237,335 +1243,343 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>166</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>73</v>
-      </c>
-      <c r="B51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" t="s">
-        <v>102</v>
+        <v>67</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>110</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
+      </c>
+      <c r="B62" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>116</v>
-      </c>
-      <c r="B65" t="s">
-        <v>117</v>
+        <v>108</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>118</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
+      </c>
+      <c r="B66" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>124</v>
-      </c>
-      <c r="B69" t="s">
-        <v>126</v>
+        <v>115</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B70" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>78</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>87</v>
-      </c>
-      <c r="B75" t="s">
-        <v>88</v>
+        <v>74</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>89</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
+      </c>
+      <c r="B76" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>90</v>
-      </c>
-      <c r="B77" t="s">
-        <v>92</v>
+        <v>83</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>95</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
+      </c>
+      <c r="B79" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>163</v>
-      </c>
-      <c r="B82" t="s">
-        <v>166</v>
-      </c>
-      <c r="C82">
-        <v>2</v>
+        <v>91</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>164</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>169</v>
+        <v>157</v>
+      </c>
+      <c r="B83" t="s">
+        <v>160</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>165</v>
-      </c>
-      <c r="B84" t="s">
-        <v>167</v>
+        <v>158</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="C84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>159</v>
+      </c>
+      <c r="B85" t="s">
+        <v>161</v>
+      </c>
+      <c r="C85">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
release build, some tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081F2F82-CBC3-489A-B304-534E295B939D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F841214F-C842-4242-86FC-60C6C11B9B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9795" yWindow="2235" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,15 +445,9 @@
     <t>intro_dialog_3</t>
   </si>
   <si>
-    <t>Multiple space blobs have pierced through our dimension!</t>
-  </si>
-  <si>
     <t>Emergency protocol initiated.</t>
   </si>
   <si>
-    <t>We must banish them immediately before they fall down to Earth!</t>
-  </si>
-  <si>
     <t>intro_attack_1</t>
   </si>
   <si>
@@ -530,6 +524,12 @@
   </si>
   <si>
     <t>Just remember to add the proper number of zeroes at the end. In this case, just a single zero.</t>
+  </si>
+  <si>
+    <t>Multiple space blobs have pierced through the sky!</t>
+  </si>
+  <si>
+    <t>We must banish them immediately before they fall down to Earth, and wreak havoc!</t>
   </si>
 </sst>
 </file>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1173,7 @@
         <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1181,39 +1181,39 @@
         <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>140</v>
       </c>
-      <c r="B38" t="s">
-        <v>143</v>
+      <c r="B38" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1237,23 +1237,23 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B45" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1261,7 +1261,7 @@
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1269,7 +1269,7 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1277,7 +1277,7 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1293,7 +1293,7 @@
         <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1301,7 +1301,7 @@
         <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1309,7 +1309,7 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1325,7 +1325,7 @@
         <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1333,7 +1333,7 @@
         <v>78</v>
       </c>
       <c r="B56" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1538,10 +1538,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C82">
         <v>2</v>
@@ -1549,21 +1549,21 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>149</v>
+      </c>
+      <c r="B84" t="s">
         <v>151</v>
-      </c>
-      <c r="B84" t="s">
-        <v>153</v>
       </c>
       <c r="C84">
         <v>4</v>

</xml_diff>

<commit_message>
added hint system for area evaluate.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F841214F-C842-4242-86FC-60C6C11B9B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1386AF-D78D-4089-91AA-E4661F2CA82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9795" yWindow="2235" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>Key</t>
   </si>
@@ -530,6 +530,66 @@
   </si>
   <si>
     <t>We must banish them immediately before they fall down to Earth, and wreak havoc!</t>
+  </si>
+  <si>
+    <t>Incorrect Multiplication: Remember that in multiples of 2, simply double the number.</t>
+  </si>
+  <si>
+    <t>Incorrect Multiplication: The trick with multiples of 3 is to double the number, and then add the original number.</t>
+  </si>
+  <si>
+    <t>Incorrect Multiplication: In multiples of 4, double the number, and then double it again.</t>
+  </si>
+  <si>
+    <t>Incorrect Multiplication: If you are having trouble with multiples of 5, try multiplying the number by 10, and then half it.</t>
+  </si>
+  <si>
+    <t>Incorrect Multiplication: A good way to solve multiples of 6 is to multiply the number by 5, and then add the original number.</t>
+  </si>
+  <si>
+    <t>Incorrect Multiplication: A good way to solve multiples of 7 is to multiply the number by 5, and then add the original number twice.</t>
+  </si>
+  <si>
+    <t>Incorrect Multiplication: If you are having trouble with multiples of 8, try multiplying the number by 2 three times.</t>
+  </si>
+  <si>
+    <t>Incorrect Multiplication: One way to do multiples of 9 is to multiply the number by 10, and then subtract it by the original number.</t>
+  </si>
+  <si>
+    <t>hint_mult_2</t>
+  </si>
+  <si>
+    <t>hint_mult_3</t>
+  </si>
+  <si>
+    <t>hint_mult_4</t>
+  </si>
+  <si>
+    <t>hint_mult_5</t>
+  </si>
+  <si>
+    <t>hint_mult_6</t>
+  </si>
+  <si>
+    <t>hint_mult_7</t>
+  </si>
+  <si>
+    <t>hint_mult_8</t>
+  </si>
+  <si>
+    <t>hint_mult_9</t>
+  </si>
+  <si>
+    <t>hint_zeroes_few</t>
+  </si>
+  <si>
+    <t>hint_zeroes_many</t>
+  </si>
+  <si>
+    <t>Incorrect number of zeroes at the end! Looks like you missed a few zeroes.</t>
+  </si>
+  <si>
+    <t>Incorrect number of zeroes at the end! Looks like you put in too many zeroes.</t>
   </si>
 </sst>
 </file>
@@ -868,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,6 +1629,116 @@
         <v>4</v>
       </c>
     </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>186</v>
+      </c>
+      <c r="B85" t="s">
+        <v>188</v>
+      </c>
+      <c r="C85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>187</v>
+      </c>
+      <c r="B86" t="s">
+        <v>189</v>
+      </c>
+      <c r="C86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>178</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C87">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" t="s">
+        <v>171</v>
+      </c>
+      <c r="C88">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>180</v>
+      </c>
+      <c r="B89" t="s">
+        <v>172</v>
+      </c>
+      <c r="C89">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" t="s">
+        <v>173</v>
+      </c>
+      <c r="C90">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" t="s">
+        <v>174</v>
+      </c>
+      <c r="C91">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" t="s">
+        <v>175</v>
+      </c>
+      <c r="C92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" t="s">
+        <v>177</v>
+      </c>
+      <c r="C94">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added digit destroyer if player is really struggling, some tweaks, update language from review.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1386AF-D78D-4089-91AA-E4661F2CA82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867F4B1B-7647-44D1-B556-14EE79404C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="2235" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8445" yWindow="2655" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>Key</t>
   </si>
@@ -590,6 +590,36 @@
   </si>
   <si>
     <t>Incorrect number of zeroes at the end! Looks like you put in too many zeroes.</t>
+  </si>
+  <si>
+    <t>digitDestroy</t>
+  </si>
+  <si>
+    <t>digitDestroy_desc</t>
+  </si>
+  <si>
+    <t>Select a blob to proceed.</t>
+  </si>
+  <si>
+    <t>Select a digit to destroy.</t>
+  </si>
+  <si>
+    <t>digitDestroy_modal_desc</t>
+  </si>
+  <si>
+    <t>digitDestroy_dialog_1</t>
+  </si>
+  <si>
+    <t>digitDestroy_dialog_2</t>
+  </si>
+  <si>
+    <t>However, this will subtract from your score, so use it sparingly!</t>
+  </si>
+  <si>
+    <t>DIGIT DESTROYER</t>
+  </si>
+  <si>
+    <t>If you are having difficulty with certain numbers, press this button to remove some of its digits.</t>
   </si>
 </sst>
 </file>
@@ -928,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,6 +1769,46 @@
         <v>8</v>
       </c>
     </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>191</v>
+      </c>
+      <c r="B96" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>194</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>195</v>
+      </c>
+      <c r="B98" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" t="s">
+        <v>197</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
updated to new unity build, updated lol api, fixed connecting wrong blobs, global pooling of blobs/connects, added way to strip coding to compensate animator, other things.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867F4B1B-7647-44D1-B556-14EE79404C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2DA4A1-8A98-4B48-AF0F-E4D63A1D1AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8445" yWindow="2655" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="2940" windowWidth="20160" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
+    <sheet name="es" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="298">
   <si>
     <t>Key</t>
   </si>
@@ -232,9 +233,6 @@
     <t>bonusBlob_1</t>
   </si>
   <si>
-    <t>Look, there’s an anomaly blob!</t>
-  </si>
-  <si>
     <t>bonusBlob_2</t>
   </si>
   <si>
@@ -244,12 +242,6 @@
     <t>bonusBlob_4</t>
   </si>
   <si>
-    <t>Connecting with this blob will allow us to clear out the entire board, and give us a bonus score.</t>
-  </si>
-  <si>
-    <t>Who knows what challenge awaits, so why not give it a try?</t>
-  </si>
-  <si>
     <t>However, you only have one shot. Do your best!</t>
   </si>
   <si>
@@ -274,15 +266,9 @@
     <t>Simply drag the numbers to their appropriate place, and once you are satisfied, press the PROCEED button.</t>
   </si>
   <si>
-    <t>Hint: If you look closely at the size of each rectangle, and its associated width, you will know where to put the numbers.</t>
-  </si>
-  <si>
     <t>bonus_partial_products_1</t>
   </si>
   <si>
-    <t>Uh oh, some of the partial products are missing!</t>
-  </si>
-  <si>
     <t>bonus_partial_products_2</t>
   </si>
   <si>
@@ -292,15 +278,9 @@
     <t>bonus_partial_products_4</t>
   </si>
   <si>
-    <t>Use the numpad to fill in the missing numbers, then press the left or right arrows to move to the next one.</t>
-  </si>
-  <si>
     <t>Once all the missing numbers are filled, press the ENTER button to proceed.</t>
   </si>
   <si>
-    <t>Just remember how you split the numbers up into multiples of 10’s like before, and you should have no problem!</t>
-  </si>
-  <si>
     <t>Finally, we add the numbers together to form the final product!</t>
   </si>
   <si>
@@ -313,9 +293,6 @@
     <t>lesson4_intro_2</t>
   </si>
   <si>
-    <t>This time around, we will be multiplying double digit numbers.</t>
-  </si>
-  <si>
     <t>lesson4_area_1</t>
   </si>
   <si>
@@ -337,9 +314,6 @@
     <t>lesson4_attack_eval_dd_1</t>
   </si>
   <si>
-    <t>This time around, you will be multiplying two double digit numbers.</t>
-  </si>
-  <si>
     <t>lesson4_attack_eval_dd_2</t>
   </si>
   <si>
@@ -511,18 +485,12 @@
     <t>To help us visualize this further, consider the factors as the dimensions of a rectangle, and the product as the area.</t>
   </si>
   <si>
-    <t>Just like in the example, this is where you split the numbers up that represents the dimensions of a rectangle.</t>
-  </si>
-  <si>
     <t>Now we compute the area of each rectangle by using the numpad to type in the number.</t>
   </si>
   <si>
     <t>Once you have a number ready, press the ENTER button.</t>
   </si>
   <si>
-    <t>Since we split the number up in multiples of 10’s, you only really have to multiply the non-zero numbers.</t>
-  </si>
-  <si>
     <t>Just remember to add the proper number of zeroes at the end. In this case, just a single zero.</t>
   </si>
   <si>
@@ -620,6 +588,333 @@
   </si>
   <si>
     <t>If you are having difficulty with certain numbers, press this button to remove some of its digits.</t>
+  </si>
+  <si>
+    <t>Just like in the example, this is where you split the numbers up that represent the dimensions of a rectangle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since we split the number up into multiples of 10, you only have to multiply the non-zero numbers. </t>
+  </si>
+  <si>
+    <t>This time around, we will be multiplying double-digit numbers.</t>
+  </si>
+  <si>
+    <t>This time around, you will be multiplying two double-digit numbers.</t>
+  </si>
+  <si>
+    <t>Look! There’s an anomaly blob!</t>
+  </si>
+  <si>
+    <t>Connecting with this blob will allow us to clear out the entire board and give us a bonus score.</t>
+  </si>
+  <si>
+    <t>Who knows what challenge awaits? So why not give it a try?</t>
+  </si>
+  <si>
+    <t>Hint: If you look closely at the size of each rectangle and its associated width, you will know where to put the numbers.</t>
+  </si>
+  <si>
+    <t>Uh oh! Some of the partial products are missing!</t>
+  </si>
+  <si>
+    <t>Use the numpad to fill in the missing numbers. Then, press the left or right arrows to move to the next one.</t>
+  </si>
+  <si>
+    <t>Just remember the way you split the numbers up into multiples of 10’s like before, and you should have no problem!</t>
+  </si>
+  <si>
+    <t>&lt;Size=50&gt;Ataca&lt;/size&gt; a Blob\nMega Multiplica</t>
+  </si>
+  <si>
+    <t>Realizado por: RENEGADEWARE, música de: Kevin MacLeod</t>
+  </si>
+  <si>
+    <t>OPCIONES</t>
+  </si>
+  <si>
+    <t>MÚSICA</t>
+  </si>
+  <si>
+    <t>SONIDO</t>
+  </si>
+  <si>
+    <t>DISCURSO</t>
+  </si>
+  <si>
+    <t>CERRAR</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>APAGADO</t>
+  </si>
+  <si>
+    <t>LISTO</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>ENTRAR</t>
+  </si>
+  <si>
+    <t>PROCEDER</t>
+  </si>
+  <si>
+    <t>VICTORIA</t>
+  </si>
+  <si>
+    <t>COMBINACIÓN</t>
+  </si>
+  <si>
+    <t>BONIFICACIÓN</t>
+  </si>
+  <si>
+    <t>PERFECTO</t>
+  </si>
+  <si>
+    <t>RESUMEN</t>
+  </si>
+  <si>
+    <t>NUEVO JUEGO</t>
+  </si>
+  <si>
+    <t>CONTINUAR</t>
+  </si>
+  <si>
+    <t>Error de multiplicación:</t>
+  </si>
+  <si>
+    <t>Error de suma:</t>
+  </si>
+  <si>
+    <t>Puntuación:</t>
+  </si>
+  <si>
+    <t>Puntuación total:</t>
+  </si>
+  <si>
+    <t>¡Cuidado! Una vez que la barra de salud esté vacía, ¡tendrás que empezar de nuevo!</t>
+  </si>
+  <si>
+    <t>Propiedad distributiva</t>
+  </si>
+  <si>
+    <t>Área del rectángulo</t>
+  </si>
+  <si>
+    <t>Nivel 1</t>
+  </si>
+  <si>
+    <t>Nivel 2</t>
+  </si>
+  <si>
+    <t>Nivel 3</t>
+  </si>
+  <si>
+    <t>Nivel 4</t>
+  </si>
+  <si>
+    <t>Inactivo</t>
+  </si>
+  <si>
+    <t>PELIGRO!!!</t>
+  </si>
+  <si>
+    <t>Atacar a Blob</t>
+  </si>
+  <si>
+    <t>¡Varias burbujas espaciales han atravesado el cielo!</t>
+  </si>
+  <si>
+    <t>Protocolo de emergencia iniciado.</t>
+  </si>
+  <si>
+    <t>¡Debemos desterrarlos inmediatamente antes de que caigan a la Tierra y causen estragos!</t>
+  </si>
+  <si>
+    <t>Con nuestros últimos avances en blobología, implementaremos Attack Blobs.</t>
+  </si>
+  <si>
+    <t>Estas manchas deben estar hechas con el poder de la multiplicación, ¡y quién mejor para hacerlo que tú!</t>
+  </si>
+  <si>
+    <t>Nuestro intrépido héroe, ¡adelante y usa tu poder matemático para desterrar estas manchas invasoras para siempre!</t>
+  </si>
+  <si>
+    <t>Multiplicar un número de dos o más dígitos puede ser complicado, ¡pero hay un truco especial para hacerlo más fácil!</t>
+  </si>
+  <si>
+    <t>Echemos un vistazo rápido a un concepto matemático que utilizaremos para este truco.</t>
+  </si>
+  <si>
+    <t>Al usar la propiedad distributiva, podemos dividir un número grande en partes más pequeñas.</t>
+  </si>
+  <si>
+    <t>En este ejemplo, dividimos el factor 12 en: 10 y 2. Facilitar la resolución del producto.</t>
+  </si>
+  <si>
+    <t>¡Presta mucha atención a cómo funciona la distribución!</t>
+  </si>
+  <si>
+    <t>Para ayudarnos a visualizar esto mejor, considera los factores como las dimensiones de un rectángulo y el producto como el área.</t>
+  </si>
+  <si>
+    <t>Dividir el rectángulo en partes más pequeñas es similar a cómo funciona la propiedad distributiva.</t>
+  </si>
+  <si>
+    <t>Luego calculamos estas áreas más pequeñas y las sumamos para obtener el área total (el producto).</t>
+  </si>
+  <si>
+    <t>Vamos a intentarlo. ¡Conecta estas dos manchas para iniciar el ataque!</t>
+  </si>
+  <si>
+    <t>Al igual que en el ejemplo, aquí es donde se dividen los números que representan las dimensiones de un rectángulo.</t>
+  </si>
+  <si>
+    <t>¡Simplemente haz clic en el número de la caja para dividirlo!</t>
+  </si>
+  <si>
+    <t>Ahora calculamos el área de cada rectángulo usando el teclado numérico para escribir el número.</t>
+  </si>
+  <si>
+    <t>Cuando tengas un número listo, pulsa el botón ENTER.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como dividimos el número en múltiplos de 10, solo tienes que multiplicar los números distintos de cero. </t>
+  </si>
+  <si>
+    <t>Solo recuerda añadir el número correcto de ceros al final. En este caso, solo un cero.</t>
+  </si>
+  <si>
+    <t>¡Finalmente, sumamos los números para formar el producto final!</t>
+  </si>
+  <si>
+    <t>Una vez más, utilice el teclado numérico para calcular cada dígito del número.</t>
+  </si>
+  <si>
+    <t>¡Excelente! Como puedes ver, es mucho más fácil resolver una ecuación dividiéndola en partes más pequeñas.</t>
+  </si>
+  <si>
+    <t>¡Ahora estás listo para desterrar las manchas!</t>
+  </si>
+  <si>
+    <t>Aquí estamos en la fase final, ¡con solo un puñado de manchas por desterrar!</t>
+  </si>
+  <si>
+    <t>Esta vez, vamos a multiplicar números de dos dígitos.</t>
+  </si>
+  <si>
+    <t>Del mismo modo que dividimos el área horizontalmente, también podemos dividirla verticalmente.</t>
+  </si>
+  <si>
+    <t>Ahora, ¿por qué no lo intentas?</t>
+  </si>
+  <si>
+    <t>Tal como lo ha hecho hasta ahora, simplemente haga clic en los números de la caja para dividirlos.</t>
+  </si>
+  <si>
+    <t>Esta vez, multiplicarás dos números de dos dígitos.</t>
+  </si>
+  <si>
+    <t>Afortunadamente, ambos son múltiplos de 10.</t>
+  </si>
+  <si>
+    <t>Todo lo que necesitas hacer es multiplicar los dos dígitos distintos de cero y poner dos ceros al final.</t>
+  </si>
+  <si>
+    <t>¡Qué bonito! Incluso multiplicando dos dígitos, ¡dividirlos te permite resolverlos con facilidad!</t>
+  </si>
+  <si>
+    <t>¡Seguro que no tendrás problemas para lidiar con las manchas restantes!</t>
+  </si>
+  <si>
+    <t>¡Mira! ¡Hay una mancha anormal!</t>
+  </si>
+  <si>
+    <t>Conectarnos con esta mancha nos permitirá limpiar todo el tablero y obtener una puntuación extra.</t>
+  </si>
+  <si>
+    <t>¿Quién sabe qué desafío nos espera? Entonces, ¿por qué no intentarlo?</t>
+  </si>
+  <si>
+    <t>Sin embargo, solo tienes una oportunidad. ¡Haz lo mejor que puedas!</t>
+  </si>
+  <si>
+    <t>¡Parece que los números de cada área están mezclados!</t>
+  </si>
+  <si>
+    <t>Simplemente arrastra los números a su lugar correspondiente y, una vez que estés satisfecho, pulsa el botón CONTINUAR.</t>
+  </si>
+  <si>
+    <t>Consejo: si observas detenidamente el tamaño de cada rectángulo y su ancho asociado, sabrás dónde colocar los números.</t>
+  </si>
+  <si>
+    <t>¡Eh, oh! ¡Faltan algunos de los productos parciales!</t>
+  </si>
+  <si>
+    <t>Usa el teclado numérico para rellenar los números que faltan. A continuación, pulsa las flechas izquierda o derecha para pasar a la siguiente.</t>
+  </si>
+  <si>
+    <t>Una vez rellenados todos los números faltantes, pulse el botón ENTER para continuar.</t>
+  </si>
+  <si>
+    <t>Solo recuerda la forma en que dividiste los números en múltiplos de 10 como antes, ¡y no deberías tener ningún problema!</t>
+  </si>
+  <si>
+    <t>ENHORABUENA!</t>
+  </si>
+  <si>
+    <t>¡Todas las manchas han sido desterradas para siempre! ¡La Tierra está a salvo una vez más!</t>
+  </si>
+  <si>
+    <t>¡Gracias por jugar!</t>
+  </si>
+  <si>
+    <t>¡Número incorrecto de ceros al final! Parece que te saltaste algunos ceros.</t>
+  </si>
+  <si>
+    <t>¡Número incorrecto de ceros al final! Parece que pusiste demasiados ceros.</t>
+  </si>
+  <si>
+    <t>Multiplicación incorrecta: Recuerda que en múltiplos de 2, simplemente dobla el número.</t>
+  </si>
+  <si>
+    <t>Multiplicación incorrecta: El truco con múltiplos de 3 consiste en doblar el número y luego sumar el número original.</t>
+  </si>
+  <si>
+    <t>Multiplicación incorrecta: en múltiplos de 4, duplica el número y vuelve a duplicarlo.</t>
+  </si>
+  <si>
+    <t>Multiplicación incorrecta: Si tienes problemas con los múltiplos de 5, intenta multiplicar el número por 10 y luego por la mitad.</t>
+  </si>
+  <si>
+    <t>Multiplicación incorrecta: una buena forma de resolver múltiplos de 6 es multiplicar el número por 5 y luego sumar el número original.</t>
+  </si>
+  <si>
+    <t>Multiplicación incorrecta: una buena forma de resolver múltiplos de 7 es multiplicar el número por 5 y luego sumar el número original dos veces.</t>
+  </si>
+  <si>
+    <t>Multiplicación incorrecta: Si tienes problemas con los múltiplos de 8, intenta multiplicar el número por 2 tres veces.</t>
+  </si>
+  <si>
+    <t>Multiplicación incorrecta: Una forma de hacer múltiplos de 9 es multiplicar el número por 10 y luego restarlo por el número original.</t>
+  </si>
+  <si>
+    <t>DESTRUCTOR DE DÍGITOS</t>
+  </si>
+  <si>
+    <t>Selecciona un blob para continuar.</t>
+  </si>
+  <si>
+    <t>Selecciona un dígito para destruirlo.</t>
+  </si>
+  <si>
+    <t>Si tiene dificultades con ciertos números, pulse este botón para eliminar algunos de sus dígitos.</t>
+  </si>
+  <si>
+    <t>Sin embargo, esto restará valor a tu puntuación, ¡así que úsala con moderación!</t>
   </si>
 </sst>
 </file>
@@ -960,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +1286,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -999,7 +1294,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1124,26 +1419,26 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1172,10 +1467,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,106 +1499,106 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B36" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B39" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1327,23 +1622,23 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B46" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1351,7 +1646,7 @@
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1359,7 +1654,7 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1367,7 +1662,7 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1383,7 +1678,7 @@
         <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1391,7 +1686,7 @@
         <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1399,7 +1694,7 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1407,23 +1702,23 @@
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B56" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1431,7 +1726,7 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1460,82 +1755,82 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B65" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>105</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B69" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B70" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1543,95 +1838,95 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>74</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>75</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>90</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>92</v>
+        <v>199</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B82" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C82">
         <v>2</v>
@@ -1639,10 +1934,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C83">
         <v>6</v>
@@ -1650,10 +1945,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B84" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C84">
         <v>4</v>
@@ -1661,10 +1956,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C85">
         <v>6</v>
@@ -1672,10 +1967,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B86" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C86">
         <v>6</v>
@@ -1683,10 +1978,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C87">
         <v>6</v>
@@ -1694,10 +1989,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B88" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C88">
         <v>8</v>
@@ -1705,10 +2000,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C89">
         <v>6</v>
@@ -1716,10 +2011,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B90" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C90">
         <v>8</v>
@@ -1727,10 +2022,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C91">
         <v>8</v>
@@ -1738,10 +2033,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B92" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C92">
         <v>8</v>
@@ -1749,10 +2044,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B93" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C93">
         <v>8</v>
@@ -1760,10 +2055,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B94" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C94">
         <v>8</v>
@@ -1771,46 +2066,904 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B95" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B96" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B97" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B98" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B99" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14903BF-85E2-4FD7-B2B1-F8C6A0501FA6}">
+  <dimension ref="A1:D99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="66.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>102</v>
+      </c>
+      <c r="B70" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>138</v>
+      </c>
+      <c r="B82" t="s">
+        <v>280</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>139</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C83">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" t="s">
+        <v>282</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" t="s">
+        <v>283</v>
+      </c>
+      <c r="C85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>176</v>
+      </c>
+      <c r="B86" t="s">
+        <v>284</v>
+      </c>
+      <c r="C86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>167</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C87">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" t="s">
+        <v>286</v>
+      </c>
+      <c r="C88">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>169</v>
+      </c>
+      <c r="B89" t="s">
+        <v>287</v>
+      </c>
+      <c r="C89">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>170</v>
+      </c>
+      <c r="B90" t="s">
+        <v>288</v>
+      </c>
+      <c r="C90">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>171</v>
+      </c>
+      <c r="B91" t="s">
+        <v>289</v>
+      </c>
+      <c r="C91">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>172</v>
+      </c>
+      <c r="B92" t="s">
+        <v>290</v>
+      </c>
+      <c r="C92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>173</v>
+      </c>
+      <c r="B93" t="s">
+        <v>291</v>
+      </c>
+      <c r="C93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" t="s">
+        <v>292</v>
+      </c>
+      <c r="C94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>179</v>
+      </c>
+      <c r="B95" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>180</v>
+      </c>
+      <c r="B96" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>183</v>
+      </c>
+      <c r="B97" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>184</v>
+      </c>
+      <c r="B98" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>185</v>
+      </c>
+      <c r="B99" t="s">
+        <v>297</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>